<commit_message>
add spinner UI chrome to show when results are loading
</commit_message>
<xml_diff>
--- a/tracking/tpivot-next-steps2017-06-19.xlsx
+++ b/tracking/tpivot-next-steps2017-06-19.xlsx
@@ -85,9 +85,6 @@
     <t>Refactor Jquery code to use module pattern, separating model operations from view operations in own name spaces to increase maintainability.</t>
   </si>
   <si>
-    <t>These sets of fns are already lexically separate. Not difficult to move into own modules.</t>
-  </si>
-  <si>
     <t>Add hook to change field list DOM on (drop in sorting bucket) and (remove from sorting bucket).</t>
   </si>
   <si>
@@ -164,6 +161,9 @@
   </si>
   <si>
     <t>Multiple columns are doable but will need to figure out how to cleanly create a query string with all column combos. See https://stackoverflow.com/questions/38696067/oracle-sql-pivot-on-multiple-columns-fields</t>
+  </si>
+  <si>
+    <t>View/model operations are already lexically separate. Not difficult to move into own modules.</t>
   </si>
 </sst>
 </file>
@@ -688,7 +688,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -727,7 +727,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="105" x14ac:dyDescent="0.25">
@@ -744,10 +744,10 @@
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
@@ -764,13 +764,13 @@
         <v>14</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
@@ -787,10 +787,10 @@
         <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="135" hidden="1" x14ac:dyDescent="0.25">
@@ -807,10 +807,10 @@
         <v>15</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:8" ht="120" hidden="1" x14ac:dyDescent="0.25">
@@ -818,7 +818,7 @@
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>15</v>
@@ -827,10 +827,10 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
@@ -847,10 +847,10 @@
         <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
@@ -867,13 +867,13 @@
         <v>14</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" ht="75" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="75" hidden="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>10</v>
       </c>
@@ -887,19 +887,19 @@
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>24</v>
-      </c>
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
@@ -907,58 +907,58 @@
         <v>15</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C11" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>26</v>
-      </c>
       <c r="F11" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E12" s="2" t="s">
-        <v>30</v>
-      </c>
       <c r="F12" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>15</v>
@@ -967,18 +967,18 @@
         <v>16</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="60" hidden="1" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>15</v>
@@ -987,10 +987,10 @@
         <v>16</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
cleanup col slicing code
</commit_message>
<xml_diff>
--- a/tracking/tpivot-next-steps2017-06-19.xlsx
+++ b/tracking/tpivot-next-steps2017-06-19.xlsx
@@ -688,7 +688,7 @@
   <dimension ref="A1:H14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -910,7 +910,7 @@
         <v>43</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="105" x14ac:dyDescent="0.25">

</xml_diff>